<commit_message>
Cpp implementation of v16.8
</commit_message>
<xml_diff>
--- a/comoOdeCpp/tests/testthat/data/templates_v16.8/Template_CoMoCOVID-19App_v17_all_interventions.xlsx
+++ b/comoOdeCpp/tests/testthat/data/templates_v16.8/Template_CoMoCOVID-19App_v17_all_interventions.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="3" lowestEdited="5" rupBuild="9302"/>
   <workbookPr/>
   <bookViews>
-    <workbookView windowWidth="23400" windowHeight="12000" tabRatio="648" firstSheet="6" activeTab="10"/>
+    <workbookView windowWidth="24375" windowHeight="12465" tabRatio="648" firstSheet="6" activeTab="10"/>
   </bookViews>
   <sheets>
     <sheet name="Int" sheetId="15" r:id="rId1"/>
@@ -4560,8 +4560,8 @@
   </sheetPr>
   <dimension ref="A1:G101"/>
   <sheetViews>
-    <sheetView zoomScale="150" zoomScaleNormal="150" topLeftCell="A5" workbookViewId="0">
-      <selection activeCell="E26" sqref="E26"/>
+    <sheetView zoomScale="150" zoomScaleNormal="150" workbookViewId="0">
+      <selection activeCell="B24" sqref="B24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.8733333333333" defaultRowHeight="15.75" outlineLevelCol="6"/>
@@ -6042,7 +6042,7 @@
   <dimension ref="A1:F40"/>
   <sheetViews>
     <sheetView zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
-      <selection activeCell="I30" sqref="I30"/>
+      <selection activeCell="C5" sqref="C5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" outlineLevelCol="5"/>
@@ -6735,8 +6735,8 @@
   </sheetPr>
   <dimension ref="A1:G92"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="150" zoomScaleNormal="150" topLeftCell="A5" workbookViewId="0">
-      <selection activeCell="A20" sqref="A20"/>
+    <sheetView tabSelected="1" zoomScale="150" zoomScaleNormal="150" workbookViewId="0">
+      <selection activeCell="F16" sqref="F16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.8733333333333" defaultRowHeight="15.75" outlineLevelCol="6"/>
@@ -6897,7 +6897,7 @@
         <v>43941</v>
       </c>
       <c r="D7" s="4">
-        <v>60</v>
+        <v>40</v>
       </c>
       <c r="E7" s="1" t="str">
         <f>IF(A7="","",VLOOKUP(A7,HIDDEN!$E$2:$F$15,2,FALSE))</f>
@@ -11018,7 +11018,7 @@
   <dimension ref="A1:F24"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="F25" sqref="F25"/>
+      <selection activeCell="B7" sqref="B7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.8733333333333" defaultRowHeight="15.75" outlineLevelCol="5"/>
@@ -12095,7 +12095,7 @@
   <dimension ref="A1:E22"/>
   <sheetViews>
     <sheetView zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
-      <selection activeCell="C20" sqref="C20"/>
+      <selection activeCell="E1" sqref="E$1:E$1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" outlineLevelCol="4"/>

</xml_diff>